<commit_message>
Update 01 Revision 01
</commit_message>
<xml_diff>
--- a/gamelogs/ben_roethlisberger.xlsx
+++ b/gamelogs/ben_roethlisberger.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdove/Desktop/Data Science/Stat231JackDove/gamelogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnkoomson/STAT231/ASSIGNMENTS/Blog-Red-Bull/gamelogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4AA34D-1E03-1B44-9921-590DA610A630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1160" windowWidth="24960" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -228,6 +229,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -495,11 +499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +538,7 @@
     <col min="29" max="29" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:99" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>